<commit_message>
Compute full flow of passangers.
</commit_message>
<xml_diff>
--- a/advance.xlsx
+++ b/advance.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>пр.Маршала Жукова (посадки нет)</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>Комсомольская пл.</t>
+  </si>
+  <si>
+    <t>ст. метро "Кировский завод"</t>
+  </si>
+  <si>
+    <t>ул. Возрождения</t>
   </si>
 </sst>
 </file>
@@ -451,15 +457,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,8 +541,14 @@
       <c r="Y1" t="s">
         <v>24</v>
       </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -611,6 +623,100 @@
       </c>
       <c r="Y2">
         <v>2.0680743243243245</v>
+      </c>
+      <c r="Z2">
+        <v>0.5778812382585965</v>
+      </c>
+      <c r="AA2">
+        <v>9.6653870238775877E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>3.35576657140223E-2</v>
+      </c>
+      <c r="C3">
+        <v>5.1995943578869726E-2</v>
+      </c>
+      <c r="D3">
+        <v>3.9826680188070437E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.10067299714206691</v>
+      </c>
+      <c r="F3">
+        <v>2.1572785101871488E-2</v>
+      </c>
+      <c r="G3">
+        <v>2.931686180510739E-2</v>
+      </c>
+      <c r="H3">
+        <v>3.5954641836452458E-2</v>
+      </c>
+      <c r="I3">
+        <v>2.8210565133216542E-2</v>
+      </c>
+      <c r="J3">
+        <v>3.8904766294828051E-2</v>
+      </c>
+      <c r="K3">
+        <v>5.0889646906978885E-2</v>
+      </c>
+      <c r="L3">
+        <v>5.7804001106296674E-2</v>
+      </c>
+      <c r="M3">
+        <v>4.9967733013736519E-2</v>
+      </c>
+      <c r="N3">
+        <v>4.3145570203742975E-2</v>
+      </c>
+      <c r="O3">
+        <v>3.4295196828616203E-2</v>
+      </c>
+      <c r="P3">
+        <v>4.2776804646446003E-2</v>
+      </c>
+      <c r="Q3">
+        <v>3.0423158476998242E-2</v>
+      </c>
+      <c r="R3">
+        <v>5.4208536922651422E-2</v>
+      </c>
+      <c r="S3">
+        <v>3.8167235180234141E-2</v>
+      </c>
+      <c r="T3">
+        <v>3.282013459942841E-2</v>
+      </c>
+      <c r="U3">
+        <v>4.1209551027933986E-2</v>
+      </c>
+      <c r="V3">
+        <v>2.9501244583755876E-3</v>
+      </c>
+      <c r="W3">
+        <v>7.1909283672904941E-3</v>
+      </c>
+      <c r="X3">
+        <v>3.0976306812943673E-2</v>
+      </c>
+      <c r="Y3">
+        <v>1.1800497833502352E-2</v>
+      </c>
+      <c r="Z3">
+        <v>7.8270489536277285E-2</v>
+      </c>
+      <c r="AA3">
+        <v>1.3091177284041668E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>7.3831304963380431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>